<commit_message>
added TMF8801 code to demonstrate isolated i2c
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C4BB808-75A3-462F-820C-7B025560BB99}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D301C-F0BE-FB42-B893-D51ADFA44CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="28600" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="ADS7952" sheetId="15" r:id="rId9"/>
     <sheet name="ADS8686" sheetId="16" r:id="rId10"/>
     <sheet name="AD7961" sheetId="13" r:id="rId11"/>
+    <sheet name="TMF8801" sheetId="17" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="322">
   <si>
     <t>Name</t>
   </si>
@@ -875,6 +876,144 @@
   </si>
   <si>
     <t>0x3F</t>
+  </si>
+  <si>
+    <t>APPID</t>
+  </si>
+  <si>
+    <t>APPREV_MAJOR</t>
+  </si>
+  <si>
+    <t>APPREQID</t>
+  </si>
+  <si>
+    <t>ENABLE</t>
+  </si>
+  <si>
+    <t>0xE0</t>
+  </si>
+  <si>
+    <t>INT_STATUS</t>
+  </si>
+  <si>
+    <t>0xE1</t>
+  </si>
+  <si>
+    <t>INT_ENAB</t>
+  </si>
+  <si>
+    <t>0xE2</t>
+  </si>
+  <si>
+    <t>0xE3</t>
+  </si>
+  <si>
+    <t>REVID</t>
+  </si>
+  <si>
+    <t>0xE4</t>
+  </si>
+  <si>
+    <t>HIST_START</t>
+  </si>
+  <si>
+    <t>HIST_END</t>
+  </si>
+  <si>
+    <t>0x9F</t>
+  </si>
+  <si>
+    <t>SERIES_NUMBER_0</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION_NUMBER_0</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION_NUMBER_1</t>
+  </si>
+  <si>
+    <t>CMD_DATA9</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>CMD_DATA0</t>
+  </si>
+  <si>
+    <t>CMD_DATA8</t>
+  </si>
+  <si>
+    <t>CMD_DATA7</t>
+  </si>
+  <si>
+    <t>CMD_DATA6</t>
+  </si>
+  <si>
+    <t>CMD_DATA5</t>
+  </si>
+  <si>
+    <t>CMD_DATA4</t>
+  </si>
+  <si>
+    <t>CMD_DATA3</t>
+  </si>
+  <si>
+    <t>CMD_DATA2</t>
+  </si>
+  <si>
+    <t>CMD_DATA1</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>PREVIOUS</t>
+  </si>
+  <si>
+    <t>APPREV_MINOR</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>APPREV_PATCH</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>REGISTER_CONTENTS</t>
+  </si>
+  <si>
+    <t>0x1E</t>
+  </si>
+  <si>
+    <t>TID</t>
+  </si>
+  <si>
+    <t>0x1F</t>
   </si>
 </sst>
 </file>
@@ -1269,16 +1408,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1437,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1378,7 +1517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1398,10 +1537,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -1413,16 +1552,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C21:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1581,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -1462,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -1482,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -1502,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -1522,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -1542,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -1562,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>207</v>
       </c>
@@ -1582,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1602,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>210</v>
       </c>
@@ -1622,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>212</v>
       </c>
@@ -1642,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -1662,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -1682,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>216</v>
       </c>
@@ -1702,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>218</v>
       </c>
@@ -1722,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>219</v>
       </c>
@@ -1742,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>221</v>
       </c>
@@ -1762,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>223</v>
       </c>
@@ -1782,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>225</v>
       </c>
@@ -1802,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>227</v>
       </c>
@@ -1822,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>230</v>
       </c>
@@ -1842,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>232</v>
       </c>
@@ -1862,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>233</v>
       </c>
@@ -1882,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>235</v>
       </c>
@@ -1902,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>237</v>
       </c>
@@ -1922,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>239</v>
       </c>
@@ -1942,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>241</v>
       </c>
@@ -1962,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>243</v>
       </c>
@@ -1982,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>245</v>
       </c>
@@ -2002,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -2022,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>249</v>
       </c>
@@ -2042,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>251</v>
       </c>
@@ -2062,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>252</v>
       </c>
@@ -2082,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>254</v>
       </c>
@@ -2102,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>256</v>
       </c>
@@ -2122,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>258</v>
       </c>
@@ -2142,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>260</v>
       </c>
@@ -2162,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>262</v>
       </c>
@@ -2182,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>264</v>
       </c>
@@ -2202,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>266</v>
       </c>
@@ -2222,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>268</v>
       </c>
@@ -2242,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>270</v>
       </c>
@@ -2262,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>272</v>
       </c>
@@ -2282,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -2312,21 +2451,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F8966C-0492-4738-84AA-AA5E0C7A41BB}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2346,7 +2485,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2366,7 +2505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2386,7 +2525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -2406,7 +2545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2426,7 +2565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2446,7 +2585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -2466,7 +2605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -2486,7 +2625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2506,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2526,7 +2665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -2546,7 +2685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -2566,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2588,6 +2727,665 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" t="s">
+        <v>297</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>313</v>
+      </c>
+      <c r="B22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B23" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>318</v>
+      </c>
+      <c r="B25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>320</v>
+      </c>
+      <c r="B26" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>288</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>289</v>
+      </c>
+      <c r="B28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2597,20 +3395,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2630,7 +3428,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -2650,7 +3448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -2670,7 +3468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -2690,7 +3488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -2723,17 +3521,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2753,7 +3551,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -2773,7 +3571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2793,7 +3591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -2813,7 +3611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2833,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -2853,7 +3651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -2873,7 +3671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -2893,7 +3691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -2913,7 +3711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2933,7 +3731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -2953,7 +3751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2973,7 +3771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -2993,7 +3791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -3013,7 +3811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -3033,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -3064,19 +3862,19 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3096,7 +3894,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3116,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3136,7 +3934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3166,19 +3964,19 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3198,7 +3996,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3218,7 +4016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3238,7 +4036,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -3258,7 +4056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -3278,7 +4076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -3298,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -3318,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3338,7 +4136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -3358,7 +4156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -3378,7 +4176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -3398,7 +4196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -3418,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -3438,7 +4236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -3458,7 +4256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -3478,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -3498,7 +4296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -3518,7 +4316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -3538,7 +4336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -3558,7 +4356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -3578,7 +4376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -3598,7 +4396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -3618,7 +4416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -3638,7 +4436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -3658,7 +4456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -3678,7 +4476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -3698,7 +4496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -3718,7 +4516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -3738,7 +4536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -3758,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -3778,7 +4576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -3798,7 +4596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -3818,7 +4616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -3838,7 +4636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -3858,7 +4656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -3892,16 +4690,16 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3921,7 +4719,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3941,7 +4739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3961,7 +4759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3981,7 +4779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4001,7 +4799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -4021,7 +4819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4041,7 +4839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -4061,7 +4859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -4081,7 +4879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -4102,7 +4900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -4122,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4142,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4162,7 +4960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -4182,7 +4980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -4202,7 +5000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -4222,7 +5020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -4242,7 +5040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -4262,7 +5060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -4282,7 +5080,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -4302,7 +5100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>191</v>
       </c>
@@ -4322,7 +5120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -4342,7 +5140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -4376,16 +5174,16 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4405,7 +5203,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -4425,7 +5223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -4445,7 +5243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -4465,7 +5263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -4485,7 +5283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4505,7 +5303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -4525,7 +5323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -4545,7 +5343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -4565,7 +5363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -4585,7 +5383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -4605,7 +5403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -4625,7 +5423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -4645,7 +5443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -4665,7 +5463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -4685,7 +5483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4705,7 +5503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4725,7 +5523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -4745,7 +5543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -4765,7 +5563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -4785,7 +5583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -4805,7 +5603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -4825,7 +5623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -4845,7 +5643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -4865,7 +5663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -4885,7 +5683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -4905,7 +5703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -4925,7 +5723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -4945,7 +5743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -4965,7 +5763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -4985,7 +5783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -5005,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -5025,7 +5823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -5045,7 +5843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -5065,7 +5863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -5085,7 +5883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -5105,7 +5903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -5139,9 +5937,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5174,9 +5972,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added TMF8801 as an extra I2C peripheral to test
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D301C-F0BE-FB42-B893-D51ADFA44CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04BEDF-BEE3-D749-BE4D-DA782594628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="28600" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="4580" yWindow="2360" windowWidth="19100" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="333">
   <si>
     <t>Name</t>
   </si>
@@ -1014,6 +1014,39 @@
   </si>
   <si>
     <t>0x1F</t>
+  </si>
+  <si>
+    <t>CPU_RESET</t>
+  </si>
+  <si>
+    <t>CPU_READY</t>
+  </si>
+  <si>
+    <t>PON</t>
+  </si>
+  <si>
+    <t>RESULT_INFO</t>
+  </si>
+  <si>
+    <t>RELIABILITY</t>
+  </si>
+  <si>
+    <t>MEAS_STATUS</t>
+  </si>
+  <si>
+    <t>SYS_CLOCK</t>
+  </si>
+  <si>
+    <t>DISTANCE_PEAK</t>
+  </si>
+  <si>
+    <t>TEMPERATURE</t>
+  </si>
+  <si>
+    <t>STATE_FIELD</t>
+  </si>
+  <si>
+    <t>0x1C</t>
   </si>
 </sst>
 </file>
@@ -2733,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2796,10 +2829,10 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2827,19 +2860,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2847,10 +2880,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -2867,10 +2900,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -2887,10 +2920,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -2907,10 +2940,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>286</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -2927,10 +2960,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -2947,10 +2980,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -2967,10 +3000,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -2987,10 +3020,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B13" t="s">
-        <v>295</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -3007,10 +3040,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -3027,10 +3060,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -3047,10 +3080,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -3067,10 +3100,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -3087,10 +3120,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -3107,10 +3140,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -3127,10 +3160,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>301</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -3147,10 +3180,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -3167,10 +3200,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B22" t="s">
-        <v>314</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -3187,19 +3220,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -3207,19 +3240,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="B24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E24">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -3227,10 +3260,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>318</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -3247,10 +3280,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -3267,10 +3300,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>321</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -3287,10 +3320,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
-        <v>290</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -3307,10 +3340,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>290</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -3330,7 +3363,7 @@
         <v>291</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>231</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -3347,10 +3380,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B31" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -3367,10 +3400,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -3382,6 +3415,226 @@
         <v>15</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>322</v>
+      </c>
+      <c r="B34" t="s">
+        <v>280</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>323</v>
+      </c>
+      <c r="B35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>324</v>
+      </c>
+      <c r="B36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>325</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>326</v>
+      </c>
+      <c r="B38" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>327</v>
+      </c>
+      <c r="B39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>329</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>16</v>
+      </c>
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>328</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>31</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" t="s">
+        <v>250</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
         <v>0</v>
       </c>
     </row>
@@ -3395,7 +3648,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5170,7 +5423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modifications to TMF8801_test file
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04BEDF-BEE3-D749-BE4D-DA782594628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9082A612-E58D-6842-A7A9-5CA9B91B2E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="2360" windowWidth="19100" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-23120" yWindow="3380" windowWidth="19100" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="333">
   <si>
     <t>Name</t>
   </si>
@@ -2766,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2809,10 +2809,10 @@
         <v>197</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2849,10 +2849,10 @@
         <v>197</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2860,10 +2860,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -2880,19 +2880,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2900,19 +2900,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2920,19 +2920,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2940,19 +2940,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>286</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2960,19 +2960,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2980,19 +2980,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -3000,19 +3000,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -3020,19 +3020,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -3040,19 +3040,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B14" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -3060,19 +3060,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -3080,19 +3080,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B16" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -3100,19 +3100,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3120,19 +3120,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B18" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3140,19 +3140,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -3160,19 +3160,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B20" t="s">
-        <v>301</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -3180,19 +3180,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -3200,19 +3200,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>314</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -3220,10 +3220,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B23" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -3240,10 +3240,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>315</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -3260,19 +3260,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>318</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -3280,19 +3280,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -3300,19 +3300,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="B27" t="s">
-        <v>321</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -3320,19 +3320,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>290</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -3340,19 +3340,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B29" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E29">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3363,16 +3363,16 @@
         <v>291</v>
       </c>
       <c r="B30" t="s">
-        <v>231</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E30">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -3380,19 +3380,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3400,19 +3400,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B32" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E32">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -3420,27 +3420,27 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>280</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D33">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B34" t="s">
         <v>280</v>
@@ -3452,15 +3452,15 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B35" t="s">
         <v>280</v>
@@ -3472,27 +3472,27 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B36" t="s">
-        <v>280</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B37" t="s">
         <v>159</v>
@@ -3509,10 +3509,10 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B38" t="s">
         <v>159</v>
@@ -3529,50 +3529,50 @@
         <v>6</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E39">
         <v>7</v>
       </c>
       <c r="F39">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E40">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -3580,19 +3580,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E41">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B42" t="s">
-        <v>250</v>
+        <v>332</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -3612,29 +3612,9 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>331</v>
-      </c>
-      <c r="B43" t="s">
-        <v>332</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="E43">
-        <v>8</v>
-      </c>
-      <c r="F43">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add class for DAC10801 and modify i2c_write_long, i2c_read_long for None register address
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9082A612-E58D-6842-A7A9-5CA9B91B2E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5F13F-E330-984D-B014-68BBE7B94FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23120" yWindow="3380" windowWidth="19100" windowHeight="20040" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="ADS8686" sheetId="16" r:id="rId10"/>
     <sheet name="AD7961" sheetId="13" r:id="rId11"/>
     <sheet name="TMF8801" sheetId="17" r:id="rId12"/>
+    <sheet name="DAC101C081" sheetId="18" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="335">
   <si>
     <t>Name</t>
   </si>
@@ -1047,13 +1048,19 @@
   </si>
   <si>
     <t>0x1C</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>DATA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1077,6 +1084,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1114,11 +1128,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2768,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -3616,6 +3631,84 @@
       </c>
       <c r="F42">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D16BBE-84DB-394B-A8D9-7783FA0567DF}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -4197,7 +4290,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modify Registers for addr=0x00 for DAC101C081
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5F13F-E330-984D-B014-68BBE7B94FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E175CB01-ED5C-3247-A435-14F810E97485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
@@ -3643,7 +3643,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3676,7 +3676,7 @@
         <v>333</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
@@ -3696,7 +3696,7 @@
         <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
correct bit index high for STATE_FIELD in TMF registers worksheet
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E175CB01-ED5C-3247-A435-14F810E97485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFAF3B-7521-1645-B647-10D15F31E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-34620" yWindow="3380" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3627,7 +3627,7 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -3642,7 +3642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D16BBE-84DB-394B-A8D9-7783FA0567DF}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated SPI clock rate in impedance analyzer example; changed DDR data_to_names for moving ADS['B'] channel to be synced with 'A'; fix bug in ADS8686 lpf Register position
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koer2434\Documents\fpga\pyripherals\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFAF3B-7521-1645-B647-10D15F31E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2DF48-9317-4225-87D8-771B41E9424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34620" yWindow="3380" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -690,9 +690,6 @@
     <t>lpf</t>
   </si>
   <si>
-    <t>0xC</t>
-  </si>
-  <si>
     <t>devID</t>
   </si>
   <si>
@@ -1054,6 +1051,9 @@
   </si>
   <si>
     <t>DATA</t>
+  </si>
+  <si>
+    <t>0xD</t>
   </si>
 </sst>
 </file>
@@ -1128,9 +1128,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1450,22 +1449,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235290A7-75FE-4F10-817B-094022AE6900}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1525,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1545,7 +1544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1584,12 +1583,6 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1600,16 +1593,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C21:C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1622,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -1649,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -1669,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -1689,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -1709,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -1729,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -1749,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>207</v>
       </c>
@@ -1769,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1789,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>210</v>
       </c>
@@ -1809,12 +1802,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>212</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>334</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1829,9 +1822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -1849,49 +1842,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>215</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>216</v>
       </c>
       <c r="B14" t="s">
         <v>159</v>
       </c>
       <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>217</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>218</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1909,129 +1902,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>220</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>221</v>
       </c>
       <c r="B17" t="s">
         <v>170</v>
       </c>
       <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>222</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>223</v>
       </c>
       <c r="B18" t="s">
         <v>160</v>
       </c>
       <c r="C18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>224</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>225</v>
       </c>
       <c r="B19" t="s">
         <v>161</v>
       </c>
       <c r="C19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>226</v>
       </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>227</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>228</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>229</v>
       </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>230</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>231</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>232</v>
       </c>
       <c r="B22" t="s">
         <v>117</v>
@@ -2049,432 +2042,432 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" t="s">
         <v>233</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>234</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>8</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>235</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>236</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>237</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>238</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>239</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>240</v>
       </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>7</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>241</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>242</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>243</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>244</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>245</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>246</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>8</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>247</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>248</v>
       </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30">
-        <v>8</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>249</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>250</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>8</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>251</v>
       </c>
-      <c r="B32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32">
-        <v>8</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>252</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>253</v>
       </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33">
-        <v>8</v>
-      </c>
-      <c r="E33">
-        <v>7</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>254</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>255</v>
       </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-      <c r="E34">
-        <v>7</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>256</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>257</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35">
-        <v>8</v>
-      </c>
-      <c r="E35">
-        <v>7</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>258</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>259</v>
       </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36">
-        <v>8</v>
-      </c>
-      <c r="E36">
-        <v>7</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>260</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>261</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
-        <v>8</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>262</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>263</v>
       </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38">
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <v>7</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>264</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>265</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>8</v>
-      </c>
-      <c r="E39">
-        <v>7</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>266</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>267</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>8</v>
-      </c>
-      <c r="E40">
-        <v>7</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>268</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>269</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>270</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>271</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42">
-        <v>8</v>
-      </c>
-      <c r="E42">
-        <v>7</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>272</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>273</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="E43">
-        <v>7</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>274</v>
-      </c>
-      <c r="B44" t="s">
-        <v>275</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -2503,17 +2496,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2526,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2553,7 +2546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2573,7 +2566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -2593,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2613,7 +2606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2633,7 +2626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -2653,7 +2646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -2673,7 +2666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2693,7 +2686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2713,7 +2706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -2733,7 +2726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -2753,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2783,17 +2776,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2813,9 +2806,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -2833,29 +2826,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>277</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>278</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2873,53 +2866,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" t="s">
         <v>279</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>280</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>281</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>282</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>283</v>
       </c>
-      <c r="B7" t="s">
-        <v>284</v>
-      </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -2933,33 +2926,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
       <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>285</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>286</v>
       </c>
-      <c r="B9" t="s">
-        <v>287</v>
-      </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -2973,9 +2966,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -2993,9 +2986,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
         <v>206</v>
@@ -3013,9 +3006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -3033,149 +3026,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>305</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>295</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>306</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>296</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>307</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>297</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>308</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>298</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>309</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>299</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>310</v>
-      </c>
-      <c r="B18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B19" t="s">
-        <v>301</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>311</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -3193,53 +3186,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>312</v>
       </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>313</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>314</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>315</v>
       </c>
-      <c r="B23" t="s">
-        <v>316</v>
-      </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
@@ -3253,53 +3246,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
       <c r="B24" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>317</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>318</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>319</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>320</v>
       </c>
-      <c r="B26" t="s">
-        <v>321</v>
-      </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
@@ -3313,52 +3306,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>288</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>289</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>290</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>291</v>
-      </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -3373,9 +3366,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s">
         <v>117</v>
@@ -3393,32 +3386,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>292</v>
       </c>
-      <c r="B31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>8</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>293</v>
-      </c>
       <c r="B32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -3433,12 +3426,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -3453,12 +3446,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -3473,12 +3466,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
@@ -3493,9 +3486,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
         <v>159</v>
@@ -3513,9 +3506,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B37" t="s">
         <v>159</v>
@@ -3533,9 +3526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B38" t="s">
         <v>159</v>
@@ -3553,9 +3546,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
@@ -3573,9 +3566,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B40" t="s">
         <v>170</v>
@@ -3593,32 +3586,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>329</v>
+      </c>
+      <c r="B41" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>330</v>
       </c>
-      <c r="B41" t="s">
-        <v>250</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>331</v>
-      </c>
-      <c r="B42" t="s">
-        <v>332</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -3646,12 +3639,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3671,14 +3664,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D2">
@@ -3691,14 +3684,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D3">
@@ -3724,17 +3717,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3754,7 +3747,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -3774,7 +3767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -3794,7 +3787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -3814,7 +3807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -3847,17 +3840,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3877,7 +3870,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3897,7 +3890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -3917,7 +3910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -3937,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3957,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -3977,7 +3970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -3997,7 +3990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -4017,7 +4010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -4037,7 +4030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -4057,7 +4050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -4077,7 +4070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4097,7 +4090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -4117,7 +4110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -4137,7 +4130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -4157,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4191,16 +4184,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4220,14 +4213,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2">
@@ -4240,7 +4233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4260,7 +4253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4293,16 +4286,16 @@
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4322,14 +4315,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D2">
@@ -4342,14 +4335,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D3">
@@ -4362,14 +4355,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
       <c r="B4" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D4">
@@ -4382,14 +4375,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D5">
@@ -4402,14 +4395,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
       <c r="B6" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D6">
@@ -4422,14 +4415,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>127</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D7">
@@ -4442,7 +4435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -4462,7 +4455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -4482,7 +4475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -4502,7 +4495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -4522,7 +4515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -4542,7 +4535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -4562,7 +4555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -4582,7 +4575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -4602,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -4622,7 +4615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -4642,7 +4635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -4662,7 +4655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -4682,7 +4675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -4702,7 +4695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -4722,7 +4715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -4742,7 +4735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -4762,7 +4755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -4782,7 +4775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -4802,7 +4795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -4822,7 +4815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -4842,7 +4835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -4862,7 +4855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -4882,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -4902,7 +4895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -4922,7 +4915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -4942,7 +4935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -4962,7 +4955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -4982,7 +4975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -5016,16 +5009,16 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5045,7 +5038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -5065,7 +5058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5085,7 +5078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5105,7 +5098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5125,7 +5118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5145,7 +5138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -5165,7 +5158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -5185,7 +5178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -5205,7 +5198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -5226,7 +5219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -5239,14 +5232,14 @@
       <c r="D11">
         <v>32</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>15</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5259,14 +5252,14 @@
       <c r="D12">
         <v>32</v>
       </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5286,7 +5279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5306,7 +5299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -5326,7 +5319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -5346,7 +5339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -5366,7 +5359,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -5386,7 +5379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -5406,7 +5399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -5426,7 +5419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>191</v>
       </c>
@@ -5446,7 +5439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -5466,7 +5459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -5500,16 +5493,16 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5529,7 +5522,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -5549,7 +5542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -5589,7 +5582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -5609,7 +5602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5629,7 +5622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -5649,7 +5642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -5669,7 +5662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5689,7 +5682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5709,7 +5702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -5729,7 +5722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -5749,7 +5742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -5769,7 +5762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -5789,7 +5782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -5809,7 +5802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -5829,7 +5822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -5849,7 +5842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -5869,7 +5862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -5889,7 +5882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5909,7 +5902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -5929,7 +5922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -5949,7 +5942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -5969,7 +5962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -5989,7 +5982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -6009,7 +6002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -6029,7 +6022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -6049,7 +6042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -6069,7 +6062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -6089,7 +6082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -6109,7 +6102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -6129,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -6149,7 +6142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -6169,7 +6162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -6189,7 +6182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -6209,7 +6202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -6229,7 +6222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -6263,9 +6256,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6298,9 +6291,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Ads sync (#19) fixes #14
* updated SPI clock rate in impedance analyzer example; changed DDR data_to_names for moving ADS['B'] channel to be synced with 'A'; fix bug in ADS8686 lpf Register position

* add flag to data_to_names to allow for analysis of old captures

* fix missing parameter for data_to_names

Co-authored-by: Abe Stroschein <69999361+Ajstros@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/covg_fpga/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koer2434\Documents\fpga\pyripherals\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFAF3B-7521-1645-B647-10D15F31E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2DF48-9317-4225-87D8-771B41E9424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34620" yWindow="3380" windowWidth="35840" windowHeight="20000" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -690,9 +690,6 @@
     <t>lpf</t>
   </si>
   <si>
-    <t>0xC</t>
-  </si>
-  <si>
     <t>devID</t>
   </si>
   <si>
@@ -1054,6 +1051,9 @@
   </si>
   <si>
     <t>DATA</t>
+  </si>
+  <si>
+    <t>0xD</t>
   </si>
 </sst>
 </file>
@@ -1128,9 +1128,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1450,22 +1449,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235290A7-75FE-4F10-817B-094022AE6900}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1525,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1545,7 +1544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1584,12 +1583,6 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1600,16 +1593,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C21:C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1622,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -1649,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -1669,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -1689,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -1709,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -1729,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -1749,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>207</v>
       </c>
@@ -1769,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1789,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>210</v>
       </c>
@@ -1809,12 +1802,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>212</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>334</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1829,9 +1822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -1849,49 +1842,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>215</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>216</v>
       </c>
       <c r="B14" t="s">
         <v>159</v>
       </c>
       <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>217</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>218</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1909,129 +1902,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>220</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>221</v>
       </c>
       <c r="B17" t="s">
         <v>170</v>
       </c>
       <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>222</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>223</v>
       </c>
       <c r="B18" t="s">
         <v>160</v>
       </c>
       <c r="C18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>224</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>225</v>
       </c>
       <c r="B19" t="s">
         <v>161</v>
       </c>
       <c r="C19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>226</v>
       </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>227</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>228</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>229</v>
       </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>230</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>231</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>232</v>
       </c>
       <c r="B22" t="s">
         <v>117</v>
@@ -2049,432 +2042,432 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" t="s">
         <v>233</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>234</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>8</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>235</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>236</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>237</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>238</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>239</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>240</v>
       </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>7</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>241</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>242</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>243</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>244</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>245</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>246</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>8</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>247</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>248</v>
       </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30">
-        <v>8</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>249</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>250</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>8</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>251</v>
       </c>
-      <c r="B32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32">
-        <v>8</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>252</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>253</v>
       </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33">
-        <v>8</v>
-      </c>
-      <c r="E33">
-        <v>7</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>254</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>255</v>
       </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-      <c r="E34">
-        <v>7</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>256</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>257</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35">
-        <v>8</v>
-      </c>
-      <c r="E35">
-        <v>7</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>258</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>259</v>
       </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36">
-        <v>8</v>
-      </c>
-      <c r="E36">
-        <v>7</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>260</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>261</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
-        <v>8</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>262</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>263</v>
       </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38">
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <v>7</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>264</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>265</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>8</v>
-      </c>
-      <c r="E39">
-        <v>7</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>266</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>267</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>8</v>
-      </c>
-      <c r="E40">
-        <v>7</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>268</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>269</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>270</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>271</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42">
-        <v>8</v>
-      </c>
-      <c r="E42">
-        <v>7</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>272</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>273</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="E43">
-        <v>7</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>274</v>
-      </c>
-      <c r="B44" t="s">
-        <v>275</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -2503,17 +2496,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2526,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2553,7 +2546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2573,7 +2566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -2593,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2613,7 +2606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2633,7 +2626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -2653,7 +2646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -2673,7 +2666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2693,7 +2686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2713,7 +2706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -2733,7 +2726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -2753,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2783,17 +2776,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2813,9 +2806,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -2833,29 +2826,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>277</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>278</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2873,53 +2866,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" t="s">
         <v>279</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>280</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>281</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>282</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>283</v>
       </c>
-      <c r="B7" t="s">
-        <v>284</v>
-      </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -2933,33 +2926,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
       <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>285</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>286</v>
       </c>
-      <c r="B9" t="s">
-        <v>287</v>
-      </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -2973,9 +2966,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -2993,9 +2986,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
         <v>206</v>
@@ -3013,9 +3006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -3033,149 +3026,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>305</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>295</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>306</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>296</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>307</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>297</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>308</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>298</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>309</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>299</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>310</v>
-      </c>
-      <c r="B18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B19" t="s">
-        <v>301</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>311</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -3193,53 +3186,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>312</v>
       </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>313</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>314</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>315</v>
       </c>
-      <c r="B23" t="s">
-        <v>316</v>
-      </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
@@ -3253,53 +3246,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
       <c r="B24" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>317</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>318</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>319</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>320</v>
       </c>
-      <c r="B26" t="s">
-        <v>321</v>
-      </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
@@ -3313,52 +3306,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>288</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>289</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>290</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>291</v>
-      </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -3373,9 +3366,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s">
         <v>117</v>
@@ -3393,32 +3386,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>292</v>
       </c>
-      <c r="B31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>8</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>293</v>
-      </c>
       <c r="B32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -3433,12 +3426,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -3453,12 +3446,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -3473,12 +3466,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
@@ -3493,9 +3486,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
         <v>159</v>
@@ -3513,9 +3506,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B37" t="s">
         <v>159</v>
@@ -3533,9 +3526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B38" t="s">
         <v>159</v>
@@ -3553,9 +3546,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
@@ -3573,9 +3566,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B40" t="s">
         <v>170</v>
@@ -3593,32 +3586,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>329</v>
+      </c>
+      <c r="B41" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>330</v>
       </c>
-      <c r="B41" t="s">
-        <v>250</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>331</v>
-      </c>
-      <c r="B42" t="s">
-        <v>332</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -3646,12 +3639,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3671,14 +3664,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D2">
@@ -3691,14 +3684,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D3">
@@ -3724,17 +3717,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3754,7 +3747,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -3774,7 +3767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -3794,7 +3787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -3814,7 +3807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -3847,17 +3840,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3877,7 +3870,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3897,7 +3890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -3917,7 +3910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -3937,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3957,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -3977,7 +3970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -3997,7 +3990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -4017,7 +4010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -4037,7 +4030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -4057,7 +4050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -4077,7 +4070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4097,7 +4090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -4117,7 +4110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -4137,7 +4130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -4157,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4191,16 +4184,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4220,14 +4213,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2">
@@ -4240,7 +4233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4260,7 +4253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4293,16 +4286,16 @@
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4322,14 +4315,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D2">
@@ -4342,14 +4335,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D3">
@@ -4362,14 +4355,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
       <c r="B4" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D4">
@@ -4382,14 +4375,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D5">
@@ -4402,14 +4395,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
       <c r="B6" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D6">
@@ -4422,14 +4415,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>127</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D7">
@@ -4442,7 +4435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -4462,7 +4455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -4482,7 +4475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -4502,7 +4495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -4522,7 +4515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -4542,7 +4535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -4562,7 +4555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -4582,7 +4575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -4602,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -4622,7 +4615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -4642,7 +4635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -4662,7 +4655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -4682,7 +4675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -4702,7 +4695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -4722,7 +4715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -4742,7 +4735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -4762,7 +4755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -4782,7 +4775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -4802,7 +4795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -4822,7 +4815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -4842,7 +4835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -4862,7 +4855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -4882,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -4902,7 +4895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -4922,7 +4915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -4942,7 +4935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -4962,7 +4955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -4982,7 +4975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -5016,16 +5009,16 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5045,7 +5038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -5065,7 +5058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5085,7 +5078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5105,7 +5098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5125,7 +5118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5145,7 +5138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -5165,7 +5158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -5185,7 +5178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -5205,7 +5198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -5226,7 +5219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -5239,14 +5232,14 @@
       <c r="D11">
         <v>32</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>15</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5259,14 +5252,14 @@
       <c r="D12">
         <v>32</v>
       </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5286,7 +5279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5306,7 +5299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -5326,7 +5319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -5346,7 +5339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -5366,7 +5359,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -5386,7 +5379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -5406,7 +5399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -5426,7 +5419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>191</v>
       </c>
@@ -5446,7 +5439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -5466,7 +5459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -5500,16 +5493,16 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5529,7 +5522,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -5549,7 +5542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -5589,7 +5582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -5609,7 +5602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5629,7 +5622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -5649,7 +5642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -5669,7 +5662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5689,7 +5682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5709,7 +5702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -5729,7 +5722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -5749,7 +5742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -5769,7 +5762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -5789,7 +5782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -5809,7 +5802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -5829,7 +5822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -5849,7 +5842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -5869,7 +5862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -5889,7 +5882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5909,7 +5902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -5929,7 +5922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -5949,7 +5942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -5969,7 +5962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -5989,7 +5982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -6009,7 +6002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -6029,7 +6022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -6049,7 +6042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -6069,7 +6062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -6089,7 +6082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -6109,7 +6102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -6129,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -6149,7 +6142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -6169,7 +6162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -6189,7 +6182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -6209,7 +6202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -6229,7 +6222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -6263,9 +6256,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6298,9 +6291,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>